<commit_message>
feat: Install the dompdf library and create a view for generating reports
</commit_message>
<xml_diff>
--- a/public/files/example-import-products_en.xlsx
+++ b/public/files/example-import-products_en.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\evertec\mercatodo\public\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59E73CEE-83C3-4546-88F4-1087AC306B37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB4A302C-370E-4C8E-85D7-2105ABFED2FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="39">
   <si>
     <t>sku</t>
   </si>
@@ -84,6 +84,66 @@
   </si>
   <si>
     <t>Images4</t>
+  </si>
+  <si>
+    <t>Information format</t>
+  </si>
+  <si>
+    <t>Field</t>
+  </si>
+  <si>
+    <t>Condition</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unique -Required in case of update - do not enter if it is a new product </t>
+  </si>
+  <si>
+    <t>Required - Unique - Alphanumeric, minimum 5 characters, maximum 10</t>
+  </si>
+  <si>
+    <t>Required - Unique - minimum 4 characters, maximum 60</t>
+  </si>
+  <si>
+    <t>Required - Unique - minimum 80 characters, maximum 400</t>
+  </si>
+  <si>
+    <t>Numerical - Greater than zero - 2 decimals - maximum 13 digits - without currency format - place price in Colombian peso (COP)</t>
+  </si>
+  <si>
+    <t>Required - One or two digit integer</t>
+  </si>
+  <si>
+    <t>Required - Put existing 'id' in category table</t>
+  </si>
+  <si>
+    <t>Required - Active or Inactive</t>
+  </si>
+  <si>
+    <t>Required - Integer - minimum zero</t>
+  </si>
+  <si>
+    <t>Public url of the image.                            Example: https://support.apple.com/library/content/dam/edam/applecare/images/es_MX/icloud/pc-ios-14-iphone-11-pro-icloud-photos-hero.jpg</t>
+  </si>
+  <si>
+    <t>https://support.apple.com/library/content/dam/edam/applecare/images/es_MX/icloud/pc-ios-14-iphone-11-pro-icloud-photos-hero.jpg</t>
+  </si>
+  <si>
+    <t>9999999</t>
+  </si>
+  <si>
+    <t>This is a example</t>
+  </si>
+  <si>
+    <t>Esto es un ejemplo</t>
+  </si>
+  <si>
+    <t>This is a example this is a example This is a example this is a exampleThis is a example this is a exampleThis is a example this is a exampleThis is a example this is a exampleThis is a example this is a exampleThis is a example this is a exampleThis is a example this is a exampleThis is a example this is a example</t>
+  </si>
+  <si>
+    <t>Esto es una ejemplo esto es una ejemplo Esto es una ejemplo esto es una ejemplo Esto es una ejemplo esto es una ejemplo Esto es una ejemplo esto es una ejemplo Esto es una ejemplo esto es una ejemplo Esto es una ejemplo esto es una ejemplo Esto es una ejemplo esto es una ejemplo</t>
+  </si>
+  <si>
+    <t>Active</t>
   </si>
   <si>
     <r>
@@ -99,7 +159,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Note</t>
+      <t>Note 1</t>
     </r>
     <r>
       <rPr>
@@ -113,64 +173,19 @@
     </r>
   </si>
   <si>
-    <t>Information format</t>
-  </si>
-  <si>
-    <t>Field</t>
-  </si>
-  <si>
-    <t>Condition</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Unique -Required in case of update - do not enter if it is a new product </t>
-  </si>
-  <si>
-    <t>Required - Unique - Alphanumeric, minimum 5 characters, maximum 10</t>
-  </si>
-  <si>
-    <t>Required - Unique - minimum 4 characters, maximum 60</t>
-  </si>
-  <si>
-    <t>Required - Unique - minimum 80 characters, maximum 400</t>
-  </si>
-  <si>
-    <t>Numerical - Greater than zero - 2 decimals - maximum 13 digits - without currency format - place price in Colombian peso (COP)</t>
-  </si>
-  <si>
-    <t>Required - One or two digit integer</t>
-  </si>
-  <si>
-    <t>Required - Put existing 'id' in category table</t>
-  </si>
-  <si>
-    <t>Required - Active or Inactive</t>
-  </si>
-  <si>
-    <t>Required - Integer - minimum zero</t>
-  </si>
-  <si>
-    <t>Public url of the image.                            Example: https://support.apple.com/library/content/dam/edam/applecare/images/es_MX/icloud/pc-ios-14-iphone-11-pro-icloud-photos-hero.jpg</t>
-  </si>
-  <si>
-    <t>https://support.apple.com/library/content/dam/edam/applecare/images/es_MX/icloud/pc-ios-14-iphone-11-pro-icloud-photos-hero.jpg</t>
-  </si>
-  <si>
-    <t>9999999</t>
-  </si>
-  <si>
-    <t>This is a example</t>
-  </si>
-  <si>
-    <t>Esto es un ejemplo</t>
-  </si>
-  <si>
-    <t>This is a example this is a example This is a example this is a exampleThis is a example this is a exampleThis is a example this is a exampleThis is a example this is a exampleThis is a example this is a exampleThis is a example this is a exampleThis is a example this is a exampleThis is a example this is a example</t>
-  </si>
-  <si>
-    <t>Esto es una ejemplo esto es una ejemplo Esto es una ejemplo esto es una ejemplo Esto es una ejemplo esto es una ejemplo Esto es una ejemplo esto es una ejemplo Esto es una ejemplo esto es una ejemplo Esto es una ejemplo esto es una ejemplo Esto es una ejemplo esto es una ejemplo</t>
-  </si>
-  <si>
-    <t>Active</t>
+    <r>
+      <t>Note 2:  C</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>opy your products to import, always from row 18, where the example record is currently located</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -250,7 +265,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -289,6 +304,9 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -575,7 +593,7 @@
   <dimension ref="A2:P18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -598,16 +616,16 @@
   <sheetData>
     <row r="2" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B2" s="11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C2" s="11"/>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="4" spans="2:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
@@ -615,10 +633,10 @@
         <v>1</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E4" s="13" t="s">
-        <v>17</v>
+        <v>37</v>
       </c>
       <c r="F4" s="13"/>
     </row>
@@ -627,20 +645,24 @@
         <v>0</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E5" s="13"/>
       <c r="F5" s="13"/>
     </row>
-    <row r="6" spans="2:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:6" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="7" t="s">
         <v>2</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="7" spans="2:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+      <c r="E6" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="F6" s="14"/>
+    </row>
+    <row r="7" spans="2:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="7" t="s">
         <v>4</v>
       </c>
@@ -651,7 +673,7 @@
         <v>3</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="2:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -665,7 +687,7 @@
         <v>6</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11" spans="2:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -673,7 +695,7 @@
         <v>7</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="12" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -681,7 +703,7 @@
         <v>8</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="13" spans="2:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -689,7 +711,7 @@
         <v>9</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="14" spans="2:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -697,7 +719,7 @@
         <v>10</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="15" spans="2:6" ht="102.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -705,7 +727,7 @@
         <v>11</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
@@ -761,19 +783,19 @@
     <row r="18" spans="1:16" ht="149.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="B18" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C18" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C18" s="4" t="s">
+      <c r="D18" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E18" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="D18" s="5" t="s">
+      <c r="F18" s="5" t="s">
         <v>35</v>
-      </c>
-      <c r="E18" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="F18" s="5" t="s">
-        <v>36</v>
       </c>
       <c r="G18" s="3">
         <v>65500.52</v>
@@ -785,27 +807,28 @@
         <v>1</v>
       </c>
       <c r="J18" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K18" s="3">
         <v>21</v>
       </c>
       <c r="L18" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="M18" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="N18" s="6"/>
       <c r="O18" s="6"/>
       <c r="P18" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="C6:C7"/>
     <mergeCell ref="C8:C9"/>
     <mergeCell ref="E4:F5"/>
+    <mergeCell ref="E6:F6"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>

</xml_diff>

<commit_message>
refactor: implement the WithMultipleSheets interface to separate the products to be imported and the format information of the fields to be imported, in different tabs, in the excel file
</commit_message>
<xml_diff>
--- a/public/files/example-import-products_en.xlsx
+++ b/public/files/example-import-products_en.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\evertec\mercatodo\public\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB4A302C-370E-4C8E-85D7-2105ABFED2FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68D6A7F2-439F-4F42-940C-07E92AB748F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Products" sheetId="1" r:id="rId1"/>
+    <sheet name="Information format" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="38">
   <si>
     <t>sku</t>
   </si>
@@ -120,9 +121,6 @@
   </si>
   <si>
     <t>Required - Integer - minimum zero</t>
-  </si>
-  <si>
-    <t>Public url of the image.                            Example: https://support.apple.com/library/content/dam/edam/applecare/images/es_MX/icloud/pc-ios-14-iphone-11-pro-icloud-photos-hero.jpg</t>
   </si>
   <si>
     <t>https://support.apple.com/library/content/dam/edam/applecare/images/es_MX/icloud/pc-ios-14-iphone-11-pro-icloud-photos-hero.jpg</t>
@@ -159,7 +157,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Note 1</t>
+      <t>Note</t>
     </r>
     <r>
       <rPr>
@@ -173,19 +171,7 @@
     </r>
   </si>
   <si>
-    <r>
-      <t>Note 2:  C</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>opy your products to import, always from row 18, where the example record is currently located</t>
-    </r>
+    <t>Public url of the image.                                                                        Example: https://support.apple.com/library/content/dam/edam/applecare/images/es_MX/icloud/pc-ios-14-iphone-11-pro-icloud-photos-hero.jpg</t>
   </si>
 </sst>
 </file>
@@ -265,7 +251,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -285,29 +271,26 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -590,10 +573,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:P18"/>
+  <dimension ref="A1:P2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -614,227 +597,245 @@
     <col min="16" max="16" width="23.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B2" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="C2" s="11"/>
-    </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B3" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C3" s="1" t="s">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" ht="149.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="4"/>
+      <c r="B2" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="G2" s="3">
+        <v>65500.52</v>
+      </c>
+      <c r="H2" s="3">
         <v>19</v>
       </c>
-    </row>
-    <row r="4" spans="2:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="7" t="s">
+      <c r="I2" s="2">
         <v>1</v>
       </c>
-      <c r="C4" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="E4" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="F4" s="13"/>
-    </row>
-    <row r="5" spans="2:6" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="C5" s="8" t="s">
+      <c r="J2" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="K2" s="3">
         <v>21</v>
       </c>
-      <c r="E5" s="13"/>
-      <c r="F5" s="13"/>
-    </row>
-    <row r="6" spans="2:6" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="C6" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="E6" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="F6" s="14"/>
-    </row>
-    <row r="7" spans="2:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" s="12"/>
-    </row>
-    <row r="8" spans="2:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="C8" s="12" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="9" spans="2:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C9" s="12"/>
-    </row>
-    <row r="10" spans="2:6" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C10" s="8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="11" spans="2:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C11" s="9" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="12" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C12" s="9" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="13" spans="2:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C13" s="9" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="14" spans="2:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C14" s="10" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="15" spans="2:6" ht="102.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C15" s="9" t="s">
+      <c r="L2" s="6" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H17" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I17" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J17" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K17" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L17" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="M17" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="N17" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="O17" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="P17" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="18" spans="1:16" ht="149.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="4"/>
-      <c r="B18" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="E18" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="F18" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="G18" s="3">
-        <v>65500.52</v>
-      </c>
-      <c r="H18" s="3">
-        <v>19</v>
-      </c>
-      <c r="I18" s="2">
-        <v>1</v>
-      </c>
-      <c r="J18" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="K18" s="3">
-        <v>21</v>
-      </c>
-      <c r="L18" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="M18" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="N18" s="6"/>
-      <c r="O18" s="6"/>
-      <c r="P18" s="6"/>
+      <c r="M2" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="N2" s="6"/>
+      <c r="O2" s="6"/>
+      <c r="P2" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="E4:F5"/>
-    <mergeCell ref="E6:F6"/>
-  </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="L18" r:id="rId1" xr:uid="{911C033A-7970-4D69-8BA6-438F9220D459}"/>
+    <hyperlink ref="L2" r:id="rId1" xr:uid="{911C033A-7970-4D69-8BA6-438F9220D459}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2002D4A-0B89-477E-9B3A-5EEC061F7899}">
+  <dimension ref="B2:F15"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="20.28515625" customWidth="1"/>
+    <col min="3" max="3" width="53.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="41.5703125" customWidth="1"/>
+    <col min="6" max="6" width="24.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B2" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="10"/>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B3" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="F4" s="13"/>
+    </row>
+    <row r="5" spans="2:6" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" s="13"/>
+      <c r="F5" s="13"/>
+    </row>
+    <row r="6" spans="2:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" s="12"/>
+      <c r="F6" s="12"/>
+    </row>
+    <row r="7" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="11"/>
+    </row>
+    <row r="8" spans="2:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="11"/>
+    </row>
+    <row r="10" spans="2:6" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6" ht="80.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="E4:F5"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="C8:C9"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>